<commit_message>
up to date 0307
</commit_message>
<xml_diff>
--- a/python-pandas/data/info_students_v1.xlsx
+++ b/python-pandas/data/info_students_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27504"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ugtomx.sharepoint.com/sites/2024-EJ-DM/Materiales de clase/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1804" documentId="13_ncr:1_{64D6DB50-DCF8-415A-AA25-A77B7F7EA109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07E0CBCF-4551-4DDE-B412-2FC8F5AC501E}"/>
+  <xr:revisionPtr revIDLastSave="1805" documentId="13_ncr:1_{64D6DB50-DCF8-415A-AA25-A77B7F7EA109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8CB2467-97FC-4FA8-9153-6F0AB8B8572B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="81">
   <si>
     <t>age</t>
   </si>
@@ -231,13 +231,61 @@
   </si>
   <si>
     <t xml:space="preserve">Pet </t>
+  </si>
+  <si>
+    <t>Francisco Montenegro</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>70 kg</t>
+  </si>
+  <si>
+    <t>Perro</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Perro, Gato</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Luis Daniel Armenta Leon</t>
+  </si>
+  <si>
+    <t>Elizabeth Cuellar</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>Perro, Gato, Conejo</t>
+  </si>
+  <si>
+    <t>Perla Maria Vidal Huichapan</t>
+  </si>
+  <si>
+    <t>1.65cm</t>
+  </si>
+  <si>
+    <t>50kg</t>
+  </si>
+  <si>
+    <t>Gato</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +358,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -337,7 +391,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -421,11 +475,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -486,16 +675,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W177"/>
+  <dimension ref="A1:W183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2591,11 +2804,11 @@
       <c r="G77" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I77" s="27" t="s">
+      <c r="I77" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J77" s="27"/>
-      <c r="K77" s="27"/>
+      <c r="J77" s="29"/>
+      <c r="K77" s="29"/>
       <c r="Q77" s="10"/>
       <c r="R77" s="9"/>
       <c r="S77" s="11"/>
@@ -2626,11 +2839,11 @@
       <c r="G78" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I78" s="27" t="s">
+      <c r="I78" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J78" s="27"/>
-      <c r="K78" s="27"/>
+      <c r="J78" s="29"/>
+      <c r="K78" s="29"/>
       <c r="Q78" s="10"/>
       <c r="R78" s="9"/>
       <c r="S78" s="11"/>
@@ -2661,11 +2874,11 @@
       <c r="G79" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I79" s="27" t="s">
+      <c r="I79" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J79" s="27"/>
-      <c r="K79" s="27"/>
+      <c r="J79" s="29"/>
+      <c r="K79" s="29"/>
       <c r="Q79" s="10"/>
       <c r="R79" s="9"/>
       <c r="S79" s="11"/>
@@ -2696,11 +2909,11 @@
       <c r="G80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I80" s="27" t="s">
+      <c r="I80" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J80" s="27"/>
-      <c r="K80" s="27"/>
+      <c r="J80" s="29"/>
+      <c r="K80" s="29"/>
       <c r="Q80" s="10"/>
       <c r="R80" s="9"/>
       <c r="S80" s="11"/>
@@ -2732,11 +2945,11 @@
         <v>11</v>
       </c>
       <c r="H81" s="7"/>
-      <c r="I81" s="27" t="s">
+      <c r="I81" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J81" s="27"/>
-      <c r="K81" s="27"/>
+      <c r="J81" s="29"/>
+      <c r="K81" s="29"/>
       <c r="Q81" s="10"/>
       <c r="R81" s="9"/>
       <c r="S81" s="11"/>
@@ -2767,11 +2980,11 @@
       <c r="G82" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I82" s="27" t="s">
+      <c r="I82" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J82" s="27"/>
-      <c r="K82" s="27"/>
+      <c r="J82" s="29"/>
+      <c r="K82" s="29"/>
       <c r="Q82" s="10"/>
       <c r="R82" s="9"/>
       <c r="S82" s="11"/>
@@ -2790,179 +3003,179 @@
       <c r="W83" s="11"/>
     </row>
     <row r="84" spans="1:23" ht="14.45" customHeight="1">
-      <c r="A84" s="29">
+      <c r="A84" s="18">
         <v>22</v>
       </c>
-      <c r="B84" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="C84" s="29">
+      <c r="B84" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" s="18">
         <v>1.72</v>
       </c>
-      <c r="D84" s="29">
+      <c r="D84" s="18">
         <v>65</v>
       </c>
-      <c r="E84" s="29">
+      <c r="E84" s="18">
         <v>8</v>
       </c>
-      <c r="F84" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G84" s="29" t="s">
+      <c r="F84" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G84" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H84" s="11"/>
-      <c r="I84" s="28" t="s">
+      <c r="I84" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J84" s="28"/>
-      <c r="K84" s="28"/>
+      <c r="J84" s="27"/>
+      <c r="K84" s="27"/>
     </row>
     <row r="85" spans="1:23">
-      <c r="A85" s="30">
+      <c r="A85" s="28">
         <v>21</v>
       </c>
-      <c r="B85" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" s="30">
+      <c r="B85" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" s="28">
         <v>1.65</v>
       </c>
-      <c r="D85" s="30">
+      <c r="D85" s="28">
         <v>66</v>
       </c>
-      <c r="E85" s="30">
+      <c r="E85" s="28">
         <v>8</v>
       </c>
-      <c r="F85" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G85" s="30" t="s">
+      <c r="F85" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G85" s="28" t="s">
         <v>11</v>
       </c>
       <c r="H85" s="11"/>
-      <c r="I85" s="28" t="s">
+      <c r="I85" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J85" s="28"/>
-      <c r="K85" s="28"/>
+      <c r="J85" s="27"/>
+      <c r="K85" s="27"/>
     </row>
     <row r="86" spans="1:23">
-      <c r="A86" s="30">
+      <c r="A86" s="28">
         <v>21</v>
       </c>
-      <c r="B86" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86" s="30">
+      <c r="B86" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="28">
         <v>1.76</v>
       </c>
-      <c r="D86" s="30">
+      <c r="D86" s="28">
         <v>73</v>
       </c>
-      <c r="E86" s="30">
+      <c r="E86" s="28">
         <v>8</v>
       </c>
-      <c r="F86" s="30" t="s">
+      <c r="F86" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G86" s="30" t="s">
+      <c r="G86" s="28" t="s">
         <v>11</v>
       </c>
       <c r="H86" s="11"/>
-      <c r="I86" s="28" t="s">
+      <c r="I86" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J86" s="28"/>
-      <c r="K86" s="28"/>
+      <c r="J86" s="27"/>
+      <c r="K86" s="27"/>
       <c r="M86" s="7"/>
     </row>
     <row r="87" spans="1:23">
-      <c r="A87" s="30">
+      <c r="A87" s="28">
         <v>21</v>
       </c>
-      <c r="B87" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C87" s="30">
+      <c r="B87" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="28">
         <v>1.8</v>
       </c>
-      <c r="D87" s="30">
+      <c r="D87" s="28">
         <v>80</v>
       </c>
-      <c r="E87" s="30">
+      <c r="E87" s="28">
         <v>8</v>
       </c>
-      <c r="F87" s="30" t="s">
+      <c r="F87" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G87" s="30" t="s">
+      <c r="G87" s="28" t="s">
         <v>11</v>
       </c>
       <c r="H87" s="11"/>
-      <c r="I87" s="28" t="s">
+      <c r="I87" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J87" s="28"/>
-      <c r="K87" s="28"/>
+      <c r="J87" s="27"/>
+      <c r="K87" s="27"/>
     </row>
     <row r="88" spans="1:23">
-      <c r="A88" s="30">
+      <c r="A88" s="28">
         <v>22</v>
       </c>
-      <c r="B88" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C88" s="30">
+      <c r="B88" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="28">
         <v>1.74</v>
       </c>
-      <c r="D88" s="30">
+      <c r="D88" s="28">
         <v>86</v>
       </c>
-      <c r="E88" s="30">
+      <c r="E88" s="28">
         <v>8</v>
       </c>
-      <c r="F88" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G88" s="30" t="s">
+      <c r="F88" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G88" s="28" t="s">
         <v>20</v>
       </c>
       <c r="H88" s="11"/>
-      <c r="I88" s="28" t="s">
+      <c r="I88" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J88" s="28"/>
-      <c r="K88" s="28"/>
+      <c r="J88" s="27"/>
+      <c r="K88" s="27"/>
     </row>
     <row r="89" spans="1:23">
-      <c r="A89" s="30">
+      <c r="A89" s="28">
         <v>21</v>
       </c>
-      <c r="B89" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C89" s="30">
+      <c r="B89" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="28">
         <v>1.7</v>
       </c>
-      <c r="D89" s="30">
+      <c r="D89" s="28">
         <v>75</v>
       </c>
-      <c r="E89" s="30">
+      <c r="E89" s="28">
         <v>8</v>
       </c>
-      <c r="F89" s="30" t="s">
+      <c r="F89" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G89" s="30" t="s">
+      <c r="G89" s="28" t="s">
         <v>20</v>
       </c>
       <c r="H89" s="11"/>
-      <c r="I89" s="28" t="s">
+      <c r="I89" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J89" s="28"/>
-      <c r="K89" s="28"/>
+      <c r="J89" s="27"/>
+      <c r="K89" s="27"/>
     </row>
     <row r="91" spans="1:23">
       <c r="A91" s="4">
@@ -4886,6 +5099,136 @@
       </c>
       <c r="K177" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11">
+      <c r="A179" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B179" s="31">
+        <v>24</v>
+      </c>
+      <c r="C179" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="D179" s="31">
+        <v>1.85</v>
+      </c>
+      <c r="E179" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F179" s="31">
+        <v>9</v>
+      </c>
+      <c r="G179" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H179" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11">
+      <c r="A180" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B180" s="34">
+        <v>23</v>
+      </c>
+      <c r="C180" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D180" s="34">
+        <v>1.65</v>
+      </c>
+      <c r="E180" s="34">
+        <v>58</v>
+      </c>
+      <c r="F180" s="34">
+        <v>9</v>
+      </c>
+      <c r="G180" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H180" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11">
+      <c r="A181" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B181" s="34">
+        <v>23</v>
+      </c>
+      <c r="C181" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D181" s="34">
+        <v>178</v>
+      </c>
+      <c r="E181" s="34">
+        <v>75</v>
+      </c>
+      <c r="F181" s="34">
+        <v>9</v>
+      </c>
+      <c r="G181" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H181" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11">
+      <c r="A182" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B182" s="34">
+        <v>23</v>
+      </c>
+      <c r="C182" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D182" s="34">
+        <v>1.53</v>
+      </c>
+      <c r="E182" s="34">
+        <v>65</v>
+      </c>
+      <c r="F182" s="34">
+        <v>9</v>
+      </c>
+      <c r="G182" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="H182" s="35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11">
+      <c r="A183" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B183" s="37">
+        <v>23</v>
+      </c>
+      <c r="C183" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D183" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="E183" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F183" s="37">
+        <v>9</v>
+      </c>
+      <c r="G183" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="H183" s="38" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4905,12 +5248,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D5F19CEBFB3EDA4D943966227C98E3A3" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="69c270c7eccf9e667a3106db520560e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48345ab7-8b49-49a1-bd22-5e9f7aa4ff19" xmlns:ns3="ab23660b-ffe1-4228-90d3-f8334d08ea58" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6638639f31b9ae8f54f7e1a10c371d6a" ns2:_="" ns3:_="">
     <xsd:import namespace="48345ab7-8b49-49a1-bd22-5e9f7aa4ff19"/>
@@ -5087,6 +5424,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5097,11 +5440,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6740EB7A-8144-4E8C-B013-A9F962EE5FA6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3633AECE-935A-488A-AAB6-EEF8BEC74D11}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3633AECE-935A-488A-AAB6-EEF8BEC74D11}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6740EB7A-8144-4E8C-B013-A9F962EE5FA6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>